<commit_message>
agrandar tablas, agregar tabla proveedores y detalle, falta cambiar main, excel e ia_anomaly
</commit_message>
<xml_diff>
--- a/data/facturas.xlsx
+++ b/data/facturas.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7df7592b1c43744/Escritorio/AIEP/Semestre 6/Automatizacion/factura_bot/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\OneDrive\Escritorio\AIEP\Semestre 6\Automatizacion\factura_bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{67623556-A899-4F3F-9DA1-C390FFB8CFFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{589E0318-EA49-47B0-AC44-11A4ECDE06D4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7770EC-6319-4335-A0AD-99B3D16A6807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
+    <workbookView xWindow="12384" yWindow="0" windowWidth="10656" windowHeight="12360" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,20 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>numero_factura</t>
   </si>
   <si>
-    <t>proveedor</t>
-  </si>
-  <si>
-    <t>monto</t>
-  </si>
-  <si>
-    <t>fecha</t>
-  </si>
-  <si>
     <t>F001</t>
   </si>
   <si>
@@ -65,9 +58,6 @@
     <t>F003</t>
   </si>
   <si>
-    <t>Proveedor X</t>
-  </si>
-  <si>
     <t>F004</t>
   </si>
   <si>
@@ -80,14 +70,89 @@
     <t>F006</t>
   </si>
   <si>
-    <t>Proveedor P</t>
+    <t>factura_numero</t>
+  </si>
+  <si>
+    <t>producto</t>
+  </si>
+  <si>
+    <t>cantidad</t>
+  </si>
+  <si>
+    <t>precio_unitario</t>
+  </si>
+  <si>
+    <t>Laptop HP</t>
+  </si>
+  <si>
+    <t>Mouse inalambrico</t>
+  </si>
+  <si>
+    <t>Monitor 24"</t>
+  </si>
+  <si>
+    <t>proveedor_id</t>
+  </si>
+  <si>
+    <t>fecha_emision</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>anomalia</t>
+  </si>
+  <si>
+    <t>comentarios</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>Proveedor D</t>
+  </si>
+  <si>
+    <t>Proveedor E</t>
+  </si>
+  <si>
+    <t>Proveedor F</t>
+  </si>
+  <si>
+    <t>rut</t>
+  </si>
+  <si>
+    <t>12.345.678-9</t>
+  </si>
+  <si>
+    <t>23.456.789-0</t>
+  </si>
+  <si>
+    <t>22.555.267-k</t>
+  </si>
+  <si>
+    <t>7.351.487-5</t>
+  </si>
+  <si>
+    <t>12.982.756-2</t>
+  </si>
+  <si>
+    <t>10.549.861-6</t>
+  </si>
+  <si>
+    <t>monto _total</t>
+  </si>
+  <si>
+    <t>sub_total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +166,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -110,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -133,14 +203,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,10 +241,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -479,117 +560,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7FCAE1-EC7B-40EC-92BC-8AF0D3824ADF}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45757</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="C3" s="2">
+        <v>45758</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45759</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>150000</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45757</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="C5" s="2">
+        <v>45760</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>45761</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1">
-        <v>200000</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45758</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9500000</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45759</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1">
-        <v>180000</v>
-      </c>
-      <c r="D5" s="2">
-        <v>45760</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1">
-        <v>180001</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45761</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1">
-        <v>280002</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="C7" s="2">
         <v>45762</v>
       </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6E1B1E-D22A-4A04-8CFF-CD030931E040}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>23000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B174994-FABB-4CA7-9490-6BF81298B274}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se adapto la tabla de excel y las posiciones al acceder, se cambio el invoice_prosessor.py y un poco de los demas
</commit_message>
<xml_diff>
--- a/data/facturas.xlsx
+++ b/data/facturas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\OneDrive\Escritorio\AIEP\Semestre 6\Automatizacion\factura_bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7770EC-6319-4335-A0AD-99B3D16A6807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4FB022-351F-47E4-908D-6653B375F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12384" yWindow="0" windowWidth="10656" windowHeight="12360" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>numero_factura</t>
   </si>
@@ -97,12 +97,6 @@
     <t>fecha_emision</t>
   </si>
   <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>anomalia</t>
-  </si>
-  <si>
     <t>comentarios</t>
   </si>
   <si>
@@ -146,6 +140,21 @@
   </si>
   <si>
     <t>sub_total</t>
+  </si>
+  <si>
+    <t>iva</t>
+  </si>
+  <si>
+    <t>monto_total</t>
+  </si>
+  <si>
+    <t>30 dias de plazo</t>
+  </si>
+  <si>
+    <t>Laptop 32" LG</t>
+  </si>
+  <si>
+    <t>subtotal_producto</t>
   </si>
 </sst>
 </file>
@@ -180,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -203,27 +212,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -241,6 +237,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>640080</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B744F3-0690-67B9-1BDC-274993914297}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6972300" y="1790700"/>
+          <a:ext cx="6210300" cy="2567940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -560,19 +622,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7FCAE1-EC7B-40EC-92BC-8AF0D3824ADF}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F2:F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="42.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -585,14 +648,8 @@
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -602,83 +659,109 @@
       <c r="C2" s="2">
         <v>45757</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
-        <v>45758</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>45759</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>45760</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
-        <v>45761</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>45762</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="C6" s="1">
+        <v>160000</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6*C6</f>
+        <v>320000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:D11" si="0">B7*C7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1">
+        <f>SUM(D1:D6)*0.19</f>
+        <v>60800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1">
+        <f>SUM(D6:D11)+D13</f>
+        <v>380800</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -712,7 +795,7 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -814,7 +897,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -827,20 +910,23 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.35">
@@ -850,8 +936,8 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>28</v>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -862,7 +948,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -873,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -881,10 +967,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -892,10 +978,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -903,10 +989,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios en la ubicacion y el formato de datos
</commit_message>
<xml_diff>
--- a/data/facturas.xlsx
+++ b/data/facturas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\OneDrive\Escritorio\AIEP\Semestre 6\Automatizacion\factura_bot\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7df7592b1c43744/Escritorio/AIEP/Semestre 6/Automatizacion/BOT-FACTURA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4FB022-351F-47E4-908D-6653B375F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{ED4FB022-351F-47E4-908D-6653B375F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{385981E6-9320-4D62-927E-5777BF81A8FD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -151,10 +151,10 @@
     <t>30 dias de plazo</t>
   </si>
   <si>
-    <t>Laptop 32" LG</t>
-  </si>
-  <si>
     <t>subtotal_producto</t>
+  </si>
+  <si>
+    <t>Cosa1</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -651,13 +651,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>45757</v>
+        <v>45767</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>36</v>
@@ -677,22 +677,22 @@
         <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>160000</v>
+        <v>20000</v>
       </c>
       <c r="D6" s="1">
         <f>B6*C6</f>
-        <v>320000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -746,7 +746,7 @@
       </c>
       <c r="D13" s="1">
         <f>SUM(D1:D6)*0.19</f>
-        <v>60800</v>
+        <v>7600</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -755,7 +755,7 @@
       </c>
       <c r="D14" s="1">
         <f>SUM(D6:D11)+D13</f>
-        <v>380800</v>
+        <v>47600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
todo listo sin interfaz
</commit_message>
<xml_diff>
--- a/data/facturas.xlsx
+++ b/data/facturas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a7df7592b1c43744/Escritorio/AIEP/Semestre 6/Automatizacion/BOT-FACTURA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{ED4FB022-351F-47E4-908D-6653B375F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{385981E6-9320-4D62-927E-5777BF81A8FD}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{ED4FB022-351F-47E4-908D-6653B375F167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A83C9640-D6F7-4B81-91EA-04BC9B3598A8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
+    <workbookView xWindow="5760" yWindow="720" windowWidth="17280" windowHeight="8880" xr2:uid="{2C52728F-D591-434E-A7FE-5CDDDFD179BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -239,70 +239,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Imagen 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54B744F3-0690-67B9-1BDC-274993914297}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="6972300" y="1790700"/>
-          <a:ext cx="6210300" cy="2567940"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -625,7 +563,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,9 +601,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-    </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>11</v>
@@ -761,7 +696,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>